<commit_message>
Changed pie chart to show Top 5 transactions by store.
</commit_message>
<xml_diff>
--- a/Assignment08/Src/Top5TransactionsByLoyaltyNumber.xlsx
+++ b/Assignment08/Src/Top5TransactionsByLoyaltyNumber.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicomp\Google Drive\Spring 2020 IS1040 Python\Week10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D4FB622-6B63-4947-B13F-325DA0E2F42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D80DA320-E100-4EB9-ABA7-91B8A0BE779F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="945" windowWidth="21600" windowHeight="14475" xr2:uid="{DB44CE58-C33F-4013-9926-DD21F362F31E}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="21648" windowHeight="13224" xr2:uid="{DB44CE58-C33F-4013-9926-DD21F362F31E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>138       </t>
   </si>
@@ -48,12 +44,27 @@
   </si>
   <si>
     <t>24        </t>
+  </si>
+  <si>
+    <t>Loyalty Number</t>
+  </si>
+  <si>
+    <t>Total Transactions</t>
+  </si>
+  <si>
+    <t>Date of Issue</t>
+  </si>
+  <si>
+    <t>Formatted Loyalty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,12 +94,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -405,73 +420,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60E24E1-133D-44BA-93C6-D5B96C140875}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="1">
         <v>87495</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C2" s="4">
         <v>39572</v>
       </c>
+      <c r="D2" s="3" t="str">
+        <f>A2&amp;" "&amp;TEXT(C2, "MM/DD/yyyy")</f>
+        <v>138        05/04/2008</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>87433</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>39523</v>
       </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" ref="D3:D6" si="0">A3&amp;" "&amp;TEXT(C3, "MM/DD/yyyy")</f>
+        <v>43.2       03/16/2008</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>87324</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>39522</v>
       </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>42.5       03/15/2008</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>87299</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>39511</v>
       </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>34         03/04/2008</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>87281</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>39501</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>24         02/23/2008</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>